<commit_message>
3ds, brick extends, discover logo
</commit_message>
<xml_diff>
--- a/src/main/java/utility/3ds.xlsx
+++ b/src/main/java/utility/3ds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\project3ds\src\main\java\utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44FF4AC4-25C6-4285-997D-EB8244E729B1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B32F7D9-6486-4F31-9764-BBF58CE59661}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20385" yWindow="-10920" windowWidth="29040" windowHeight="15840" xr2:uid="{BEB352CC-697D-4552-A491-A957F90EFDC3}"/>
+    <workbookView xWindow="20385" yWindow="-10920" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BEB352CC-697D-4552-A491-A957F90EFDC3}"/>
   </bookViews>
   <sheets>
     <sheet name="card" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
   <si>
     <t>cc_emcabarlero</t>
   </si>
@@ -118,6 +118,12 @@
   </si>
   <si>
     <t>isBrickToFPCustom</t>
+  </si>
+  <si>
+    <t>*Browser</t>
+  </si>
+  <si>
+    <t>IE11/FF/Chrome</t>
   </si>
 </sst>
 </file>
@@ -487,7 +493,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D26F539-7243-4AD2-9696-1C27A04624AA}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
@@ -667,10 +673,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B1143D-A132-4F80-98C2-EB689D20A65C}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,6 +828,14 @@
         <v>12</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
update framework and update test logo yandex
</commit_message>
<xml_diff>
--- a/src/main/java/utility/3ds.xlsx
+++ b/src/main/java/utility/3ds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\project3ds\src\main\java\utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B32F7D9-6486-4F31-9764-BBF58CE59661}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A75A2DF-B6DB-4291-B6BE-985F50A0BBA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20385" yWindow="-10920" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BEB352CC-697D-4552-A491-A957F90EFDC3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
   <si>
     <t>cc_emcabarlero</t>
   </si>
@@ -57,9 +57,6 @@
     <t>cc_leavenworth</t>
   </si>
   <si>
-    <t>oldwidget</t>
-  </si>
-  <si>
     <t>fasterpayproxyHtml</t>
   </si>
   <si>
@@ -124,6 +121,12 @@
   </si>
   <si>
     <t>IE11/FF/Chrome</t>
+  </si>
+  <si>
+    <t>oldwidget (widget_css_v2)</t>
+  </si>
+  <si>
+    <t>oldwidget (cc_new":1,"cc_compact":1,)</t>
   </si>
 </sst>
 </file>
@@ -511,36 +514,36 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>25</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>26</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>27</v>
-      </c>
-      <c r="H1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -563,10 +566,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -589,7 +592,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -615,7 +618,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -641,7 +644,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -673,15 +676,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B1143D-A132-4F80-98C2-EB689D20A65C}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
@@ -690,7 +693,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -710,130 +713,150 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>30</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update multiple ps smoke test
</commit_message>
<xml_diff>
--- a/src/main/java/utility/3ds.xlsx
+++ b/src/main/java/utility/3ds.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\project3ds\src\main\java\utility\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A75A2DF-B6DB-4291-B6BE-985F50A0BBA1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4DE411-6112-4C55-A740-671C5DEA4BFF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20385" yWindow="-10920" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{BEB352CC-697D-4552-A491-A957F90EFDC3}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="33">
   <si>
     <t>cc_emcabarlero</t>
   </si>
@@ -45,9 +45,6 @@
     <t>ccbarzilhipercard</t>
   </si>
   <si>
-    <t>brickwidget</t>
-  </si>
-  <si>
     <t>brickcustom</t>
   </si>
   <si>
@@ -123,17 +120,23 @@
     <t>IE11/FF/Chrome</t>
   </si>
   <si>
-    <t>oldwidget (widget_css_v2)</t>
-  </si>
-  <si>
-    <t>oldwidget (cc_new":1,"cc_compact":1,)</t>
+    <t>brick_widget</t>
+  </si>
+  <si>
+    <t>old_widget ("cc_new":1)</t>
+  </si>
+  <si>
+    <t>compact_widget ("cc_new":1,"cc_compact":1,)</t>
+  </si>
+  <si>
+    <t>custom_widget</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -144,6 +147,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -175,11 +184,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,7 +507,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,36 +524,36 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -566,10 +576,10 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -592,7 +602,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
@@ -618,7 +628,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
         <v>2</v>
@@ -644,7 +654,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>
@@ -676,15 +686,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84B1143D-A132-4F80-98C2-EB689D20A65C}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
@@ -693,7 +703,7 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -708,155 +718,175 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
+      <c r="A2" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>